<commit_message>
Nuevo Doc Issuer WebService
</commit_message>
<xml_diff>
--- a/2024 Formularios de Autorización de Acceso a Sitio en Red Interna.xlsx
+++ b/2024 Formularios de Autorización de Acceso a Sitio en Red Interna.xlsx
@@ -229,7 +229,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Samuel Armando Menendez </t>
+    <t xml:space="preserve">Caty Eloisa Zepeda</t>
   </si>
   <si>
     <r>
@@ -530,7 +530,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="29">
+  <fonts count="30">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -668,6 +668,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -965,11 +971,15 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="19" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -981,7 +991,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -989,7 +999,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -997,7 +1007,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="2" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="22" fillId="2" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1017,15 +1027,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="24" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1033,7 +1035,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="26" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="26" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1042,6 +1044,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="28" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="29" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1134,9 +1140,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>9720</xdr:colOff>
+      <xdr:colOff>9360</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>126000</xdr:rowOff>
+      <xdr:rowOff>125640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1156,7 +1162,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4418640" y="4061880"/>
-          <a:ext cx="2488320" cy="274320"/>
+          <a:ext cx="2487960" cy="273960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1182,9 +1188,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>35</xdr:col>
-      <xdr:colOff>91440</xdr:colOff>
+      <xdr:colOff>91080</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>70200</xdr:rowOff>
+      <xdr:rowOff>69840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1204,7 +1210,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3565440" y="9458280"/>
-          <a:ext cx="2320200" cy="279720"/>
+          <a:ext cx="2319840" cy="279360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1497,8 +1503,8 @@
   </sheetPr>
   <dimension ref="A2:AL131"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A16" colorId="64" zoomScale="140" zoomScaleNormal="100" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AO33" activeCellId="0" sqref="AO33"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="100" zoomScalePageLayoutView="140" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AG4" activeCellId="0" sqref="AG4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.2890625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1638,7 +1644,7 @@
       <c r="AE4" s="15"/>
       <c r="AF4" s="15"/>
       <c r="AG4" s="16" t="n">
-        <v>45770</v>
+        <v>46017</v>
       </c>
       <c r="AH4" s="16"/>
       <c r="AI4" s="16"/>
@@ -1891,75 +1897,75 @@
       <c r="M22" s="19"/>
       <c r="N22" s="19"/>
       <c r="O22" s="19"/>
-      <c r="P22" s="20" t="s">
+      <c r="P22" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="Q22" s="20"/>
-      <c r="R22" s="20"/>
-      <c r="S22" s="20"/>
-      <c r="T22" s="20"/>
-      <c r="U22" s="20"/>
-      <c r="V22" s="20"/>
-      <c r="W22" s="20"/>
-      <c r="X22" s="20"/>
-      <c r="Y22" s="20"/>
-      <c r="Z22" s="20"/>
-      <c r="AA22" s="20"/>
-      <c r="AB22" s="20"/>
-      <c r="AC22" s="20"/>
-      <c r="AD22" s="20"/>
-      <c r="AE22" s="20"/>
-      <c r="AF22" s="20"/>
-      <c r="AG22" s="20"/>
-      <c r="AH22" s="20"/>
-      <c r="AI22" s="20"/>
-      <c r="AJ22" s="20"/>
+      <c r="Q22" s="22"/>
+      <c r="R22" s="22"/>
+      <c r="S22" s="22"/>
+      <c r="T22" s="22"/>
+      <c r="U22" s="22"/>
+      <c r="V22" s="22"/>
+      <c r="W22" s="22"/>
+      <c r="X22" s="22"/>
+      <c r="Y22" s="22"/>
+      <c r="Z22" s="22"/>
+      <c r="AA22" s="22"/>
+      <c r="AB22" s="22"/>
+      <c r="AC22" s="22"/>
+      <c r="AD22" s="22"/>
+      <c r="AE22" s="22"/>
+      <c r="AF22" s="22"/>
+      <c r="AG22" s="22"/>
+      <c r="AH22" s="22"/>
+      <c r="AI22" s="22"/>
+      <c r="AJ22" s="22"/>
     </row>
     <row r="23" customFormat="false" ht="8.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="P23" s="22"/>
-      <c r="Q23" s="22"/>
-      <c r="R23" s="22"/>
-      <c r="S23" s="22"/>
-      <c r="T23" s="22"/>
-      <c r="U23" s="22"/>
-      <c r="V23" s="22"/>
-      <c r="W23" s="22"/>
-      <c r="X23" s="22"/>
-      <c r="Y23" s="22"/>
-      <c r="Z23" s="22"/>
-      <c r="AA23" s="22"/>
-      <c r="AB23" s="22"/>
-      <c r="AC23" s="22"/>
-      <c r="AD23" s="22"/>
-      <c r="AE23" s="22"/>
-      <c r="AF23" s="22"/>
-      <c r="AG23" s="22"/>
-      <c r="AH23" s="22"/>
-      <c r="AI23" s="22"/>
-      <c r="AJ23" s="22"/>
+      <c r="P23" s="23"/>
+      <c r="Q23" s="23"/>
+      <c r="R23" s="23"/>
+      <c r="S23" s="23"/>
+      <c r="T23" s="23"/>
+      <c r="U23" s="23"/>
+      <c r="V23" s="23"/>
+      <c r="W23" s="23"/>
+      <c r="X23" s="23"/>
+      <c r="Y23" s="23"/>
+      <c r="Z23" s="23"/>
+      <c r="AA23" s="23"/>
+      <c r="AB23" s="23"/>
+      <c r="AC23" s="23"/>
+      <c r="AD23" s="23"/>
+      <c r="AE23" s="23"/>
+      <c r="AF23" s="23"/>
+      <c r="AG23" s="23"/>
+      <c r="AH23" s="23"/>
+      <c r="AI23" s="23"/>
+      <c r="AJ23" s="23"/>
     </row>
     <row r="24" customFormat="false" ht="8.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="P24" s="22"/>
-      <c r="Q24" s="22"/>
-      <c r="R24" s="22"/>
-      <c r="S24" s="22"/>
-      <c r="T24" s="22"/>
-      <c r="U24" s="22"/>
-      <c r="V24" s="22"/>
-      <c r="W24" s="22"/>
-      <c r="X24" s="22"/>
-      <c r="Y24" s="22"/>
-      <c r="Z24" s="22"/>
-      <c r="AA24" s="22"/>
-      <c r="AB24" s="22"/>
-      <c r="AC24" s="22"/>
-      <c r="AD24" s="22"/>
-      <c r="AE24" s="22"/>
-      <c r="AF24" s="22"/>
-      <c r="AG24" s="22"/>
-      <c r="AH24" s="22"/>
-      <c r="AI24" s="22"/>
-      <c r="AJ24" s="22"/>
+      <c r="P24" s="23"/>
+      <c r="Q24" s="23"/>
+      <c r="R24" s="23"/>
+      <c r="S24" s="23"/>
+      <c r="T24" s="23"/>
+      <c r="U24" s="23"/>
+      <c r="V24" s="23"/>
+      <c r="W24" s="23"/>
+      <c r="X24" s="23"/>
+      <c r="Y24" s="23"/>
+      <c r="Z24" s="23"/>
+      <c r="AA24" s="23"/>
+      <c r="AB24" s="23"/>
+      <c r="AC24" s="23"/>
+      <c r="AD24" s="23"/>
+      <c r="AE24" s="23"/>
+      <c r="AF24" s="23"/>
+      <c r="AG24" s="23"/>
+      <c r="AH24" s="23"/>
+      <c r="AI24" s="23"/>
+      <c r="AJ24" s="23"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C25" s="19" t="s">
@@ -1977,35 +1983,35 @@
       <c r="M25" s="19"/>
       <c r="N25" s="19"/>
       <c r="O25" s="19"/>
-      <c r="P25" s="23" t="s">
+      <c r="P25" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="Q25" s="23"/>
-      <c r="R25" s="23"/>
-      <c r="S25" s="23"/>
-      <c r="T25" s="24" t="s">
+      <c r="Q25" s="24"/>
+      <c r="R25" s="24"/>
+      <c r="S25" s="24"/>
+      <c r="T25" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="U25" s="24"/>
-      <c r="V25" s="24"/>
-      <c r="W25" s="24"/>
-      <c r="X25" s="24"/>
-      <c r="Y25" s="24"/>
-      <c r="Z25" s="24"/>
-      <c r="AA25" s="23" t="s">
+      <c r="U25" s="25"/>
+      <c r="V25" s="25"/>
+      <c r="W25" s="25"/>
+      <c r="X25" s="25"/>
+      <c r="Y25" s="25"/>
+      <c r="Z25" s="25"/>
+      <c r="AA25" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="AB25" s="23"/>
-      <c r="AC25" s="23"/>
-      <c r="AD25" s="23"/>
-      <c r="AE25" s="25" t="s">
+      <c r="AB25" s="24"/>
+      <c r="AC25" s="24"/>
+      <c r="AD25" s="24"/>
+      <c r="AE25" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="AF25" s="25"/>
-      <c r="AG25" s="25"/>
-      <c r="AH25" s="25"/>
-      <c r="AI25" s="25"/>
-      <c r="AJ25" s="25"/>
+      <c r="AF25" s="26"/>
+      <c r="AG25" s="26"/>
+      <c r="AH25" s="26"/>
+      <c r="AI25" s="26"/>
+      <c r="AJ25" s="26"/>
     </row>
     <row r="26" customFormat="false" ht="6.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2022,32 +2028,32 @@
       <c r="M27" s="19"/>
       <c r="N27" s="19"/>
       <c r="O27" s="19"/>
-      <c r="P27" s="23" t="s">
+      <c r="P27" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="Q27" s="23"/>
-      <c r="R27" s="23"/>
-      <c r="S27" s="23"/>
-      <c r="T27" s="24" t="s">
+      <c r="Q27" s="24"/>
+      <c r="R27" s="24"/>
+      <c r="S27" s="24"/>
+      <c r="T27" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="U27" s="24"/>
-      <c r="V27" s="24"/>
-      <c r="W27" s="24"/>
-      <c r="X27" s="24"/>
-      <c r="Y27" s="24"/>
-      <c r="Z27" s="24"/>
-      <c r="AA27" s="26"/>
-      <c r="AB27" s="26"/>
-      <c r="AC27" s="26"/>
-      <c r="AD27" s="26"/>
-      <c r="AE27" s="26"/>
-      <c r="AF27" s="26"/>
-      <c r="AG27" s="26"/>
-      <c r="AH27" s="26"/>
-      <c r="AI27" s="26"/>
-      <c r="AJ27" s="26"/>
-      <c r="AK27" s="26"/>
+      <c r="U27" s="25"/>
+      <c r="V27" s="25"/>
+      <c r="W27" s="25"/>
+      <c r="X27" s="25"/>
+      <c r="Y27" s="25"/>
+      <c r="Z27" s="25"/>
+      <c r="AA27" s="27"/>
+      <c r="AB27" s="27"/>
+      <c r="AC27" s="27"/>
+      <c r="AD27" s="27"/>
+      <c r="AE27" s="27"/>
+      <c r="AF27" s="27"/>
+      <c r="AG27" s="27"/>
+      <c r="AH27" s="27"/>
+      <c r="AI27" s="27"/>
+      <c r="AJ27" s="27"/>
+      <c r="AK27" s="27"/>
     </row>
     <row r="28" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2066,183 +2072,183 @@
       <c r="M29" s="19"/>
       <c r="N29" s="19"/>
       <c r="O29" s="19"/>
-      <c r="P29" s="27" t="s">
+      <c r="P29" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="Q29" s="27"/>
-      <c r="R29" s="27"/>
-      <c r="S29" s="27"/>
-      <c r="T29" s="27"/>
-      <c r="U29" s="27"/>
-      <c r="V29" s="27"/>
-      <c r="W29" s="27"/>
-      <c r="X29" s="27"/>
-      <c r="Y29" s="27"/>
-      <c r="Z29" s="27"/>
-      <c r="AA29" s="27"/>
-      <c r="AB29" s="27"/>
-      <c r="AC29" s="27"/>
-      <c r="AD29" s="27"/>
-      <c r="AE29" s="27"/>
-      <c r="AF29" s="27"/>
-      <c r="AG29" s="27"/>
-      <c r="AH29" s="27"/>
-      <c r="AI29" s="27"/>
-      <c r="AJ29" s="27"/>
+      <c r="Q29" s="28"/>
+      <c r="R29" s="28"/>
+      <c r="S29" s="28"/>
+      <c r="T29" s="28"/>
+      <c r="U29" s="28"/>
+      <c r="V29" s="28"/>
+      <c r="W29" s="28"/>
+      <c r="X29" s="28"/>
+      <c r="Y29" s="28"/>
+      <c r="Z29" s="28"/>
+      <c r="AA29" s="28"/>
+      <c r="AB29" s="28"/>
+      <c r="AC29" s="28"/>
+      <c r="AD29" s="28"/>
+      <c r="AE29" s="28"/>
+      <c r="AF29" s="28"/>
+      <c r="AG29" s="28"/>
+      <c r="AH29" s="28"/>
+      <c r="AI29" s="28"/>
+      <c r="AJ29" s="28"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C30" s="28" t="s">
+      <c r="C30" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="D30" s="28"/>
-      <c r="E30" s="28"/>
-      <c r="F30" s="28"/>
-      <c r="G30" s="28"/>
-      <c r="H30" s="28"/>
-      <c r="I30" s="28"/>
-      <c r="J30" s="28"/>
-      <c r="K30" s="28"/>
-      <c r="L30" s="28"/>
-      <c r="M30" s="28"/>
-      <c r="N30" s="29"/>
-      <c r="P30" s="27"/>
-      <c r="Q30" s="27"/>
-      <c r="R30" s="27"/>
-      <c r="S30" s="27"/>
-      <c r="T30" s="27"/>
-      <c r="U30" s="27"/>
-      <c r="V30" s="27"/>
-      <c r="W30" s="27"/>
-      <c r="X30" s="27"/>
-      <c r="Y30" s="27"/>
-      <c r="Z30" s="27"/>
-      <c r="AA30" s="27"/>
-      <c r="AB30" s="27"/>
-      <c r="AC30" s="27"/>
-      <c r="AD30" s="27"/>
-      <c r="AE30" s="27"/>
-      <c r="AF30" s="27"/>
-      <c r="AG30" s="27"/>
-      <c r="AH30" s="27"/>
-      <c r="AI30" s="27"/>
-      <c r="AJ30" s="27"/>
+      <c r="D30" s="29"/>
+      <c r="E30" s="29"/>
+      <c r="F30" s="29"/>
+      <c r="G30" s="29"/>
+      <c r="H30" s="29"/>
+      <c r="I30" s="29"/>
+      <c r="J30" s="29"/>
+      <c r="K30" s="29"/>
+      <c r="L30" s="29"/>
+      <c r="M30" s="29"/>
+      <c r="N30" s="30"/>
+      <c r="P30" s="28"/>
+      <c r="Q30" s="28"/>
+      <c r="R30" s="28"/>
+      <c r="S30" s="28"/>
+      <c r="T30" s="28"/>
+      <c r="U30" s="28"/>
+      <c r="V30" s="28"/>
+      <c r="W30" s="28"/>
+      <c r="X30" s="28"/>
+      <c r="Y30" s="28"/>
+      <c r="Z30" s="28"/>
+      <c r="AA30" s="28"/>
+      <c r="AB30" s="28"/>
+      <c r="AC30" s="28"/>
+      <c r="AD30" s="28"/>
+      <c r="AE30" s="28"/>
+      <c r="AF30" s="28"/>
+      <c r="AG30" s="28"/>
+      <c r="AH30" s="28"/>
+      <c r="AI30" s="28"/>
+      <c r="AJ30" s="28"/>
     </row>
     <row r="31" customFormat="false" ht="53.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C31" s="28"/>
-      <c r="D31" s="28"/>
-      <c r="E31" s="28"/>
-      <c r="F31" s="28"/>
-      <c r="G31" s="28"/>
-      <c r="H31" s="28"/>
-      <c r="I31" s="28"/>
-      <c r="J31" s="28"/>
-      <c r="K31" s="28"/>
-      <c r="L31" s="28"/>
-      <c r="M31" s="28"/>
-      <c r="N31" s="29"/>
-      <c r="P31" s="27"/>
-      <c r="Q31" s="27"/>
-      <c r="R31" s="27"/>
-      <c r="S31" s="27"/>
-      <c r="T31" s="27"/>
-      <c r="U31" s="27"/>
-      <c r="V31" s="27"/>
-      <c r="W31" s="27"/>
-      <c r="X31" s="27"/>
-      <c r="Y31" s="27"/>
-      <c r="Z31" s="27"/>
-      <c r="AA31" s="27"/>
-      <c r="AB31" s="27"/>
-      <c r="AC31" s="27"/>
-      <c r="AD31" s="27"/>
-      <c r="AE31" s="27"/>
-      <c r="AF31" s="27"/>
-      <c r="AG31" s="27"/>
-      <c r="AH31" s="27"/>
-      <c r="AI31" s="27"/>
-      <c r="AJ31" s="27"/>
+      <c r="C31" s="29"/>
+      <c r="D31" s="29"/>
+      <c r="E31" s="29"/>
+      <c r="F31" s="29"/>
+      <c r="G31" s="29"/>
+      <c r="H31" s="29"/>
+      <c r="I31" s="29"/>
+      <c r="J31" s="29"/>
+      <c r="K31" s="29"/>
+      <c r="L31" s="29"/>
+      <c r="M31" s="29"/>
+      <c r="N31" s="30"/>
+      <c r="P31" s="28"/>
+      <c r="Q31" s="28"/>
+      <c r="R31" s="28"/>
+      <c r="S31" s="28"/>
+      <c r="T31" s="28"/>
+      <c r="U31" s="28"/>
+      <c r="V31" s="28"/>
+      <c r="W31" s="28"/>
+      <c r="X31" s="28"/>
+      <c r="Y31" s="28"/>
+      <c r="Z31" s="28"/>
+      <c r="AA31" s="28"/>
+      <c r="AB31" s="28"/>
+      <c r="AC31" s="28"/>
+      <c r="AD31" s="28"/>
+      <c r="AE31" s="28"/>
+      <c r="AF31" s="28"/>
+      <c r="AG31" s="28"/>
+      <c r="AH31" s="28"/>
+      <c r="AI31" s="28"/>
+      <c r="AJ31" s="28"/>
     </row>
     <row r="32" customFormat="false" ht="42" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="P32" s="27"/>
-      <c r="Q32" s="27"/>
-      <c r="R32" s="27"/>
-      <c r="S32" s="27"/>
-      <c r="T32" s="27"/>
-      <c r="U32" s="27"/>
-      <c r="V32" s="27"/>
-      <c r="W32" s="27"/>
-      <c r="X32" s="27"/>
-      <c r="Y32" s="27"/>
-      <c r="Z32" s="27"/>
-      <c r="AA32" s="27"/>
-      <c r="AB32" s="27"/>
-      <c r="AC32" s="27"/>
-      <c r="AD32" s="27"/>
-      <c r="AE32" s="27"/>
-      <c r="AF32" s="27"/>
-      <c r="AG32" s="27"/>
-      <c r="AH32" s="27"/>
-      <c r="AI32" s="27"/>
-      <c r="AJ32" s="27"/>
+      <c r="P32" s="28"/>
+      <c r="Q32" s="28"/>
+      <c r="R32" s="28"/>
+      <c r="S32" s="28"/>
+      <c r="T32" s="28"/>
+      <c r="U32" s="28"/>
+      <c r="V32" s="28"/>
+      <c r="W32" s="28"/>
+      <c r="X32" s="28"/>
+      <c r="Y32" s="28"/>
+      <c r="Z32" s="28"/>
+      <c r="AA32" s="28"/>
+      <c r="AB32" s="28"/>
+      <c r="AC32" s="28"/>
+      <c r="AD32" s="28"/>
+      <c r="AE32" s="28"/>
+      <c r="AF32" s="28"/>
+      <c r="AG32" s="28"/>
+      <c r="AH32" s="28"/>
+      <c r="AI32" s="28"/>
+      <c r="AJ32" s="28"/>
     </row>
     <row r="33" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="P33" s="27"/>
-      <c r="Q33" s="27"/>
-      <c r="R33" s="27"/>
-      <c r="S33" s="27"/>
-      <c r="T33" s="27"/>
-      <c r="U33" s="27"/>
-      <c r="V33" s="27"/>
-      <c r="W33" s="27"/>
-      <c r="X33" s="27"/>
-      <c r="Y33" s="27"/>
-      <c r="Z33" s="27"/>
-      <c r="AA33" s="27"/>
-      <c r="AB33" s="27"/>
-      <c r="AC33" s="27"/>
-      <c r="AD33" s="27"/>
-      <c r="AE33" s="27"/>
-      <c r="AF33" s="27"/>
-      <c r="AG33" s="27"/>
-      <c r="AH33" s="27"/>
-      <c r="AI33" s="27"/>
-      <c r="AJ33" s="27"/>
+      <c r="P33" s="28"/>
+      <c r="Q33" s="28"/>
+      <c r="R33" s="28"/>
+      <c r="S33" s="28"/>
+      <c r="T33" s="28"/>
+      <c r="U33" s="28"/>
+      <c r="V33" s="28"/>
+      <c r="W33" s="28"/>
+      <c r="X33" s="28"/>
+      <c r="Y33" s="28"/>
+      <c r="Z33" s="28"/>
+      <c r="AA33" s="28"/>
+      <c r="AB33" s="28"/>
+      <c r="AC33" s="28"/>
+      <c r="AD33" s="28"/>
+      <c r="AE33" s="28"/>
+      <c r="AF33" s="28"/>
+      <c r="AG33" s="28"/>
+      <c r="AH33" s="28"/>
+      <c r="AI33" s="28"/>
+      <c r="AJ33" s="28"/>
     </row>
     <row r="34" customFormat="false" ht="6.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="X35" s="30" t="s">
+      <c r="X35" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="Y35" s="30"/>
-      <c r="Z35" s="30"/>
-      <c r="AA35" s="30"/>
-      <c r="AB35" s="30"/>
-      <c r="AC35" s="30"/>
-      <c r="AD35" s="30"/>
-      <c r="AF35" s="31" t="s">
+      <c r="Y35" s="31"/>
+      <c r="Z35" s="31"/>
+      <c r="AA35" s="31"/>
+      <c r="AB35" s="31"/>
+      <c r="AC35" s="31"/>
+      <c r="AD35" s="31"/>
+      <c r="AF35" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="AG35" s="31"/>
-      <c r="AH35" s="31"/>
-      <c r="AI35" s="31"/>
-      <c r="AJ35" s="31"/>
+      <c r="AG35" s="32"/>
+      <c r="AH35" s="32"/>
+      <c r="AI35" s="32"/>
+      <c r="AJ35" s="32"/>
     </row>
     <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C36" s="32" t="s">
+      <c r="C36" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="D36" s="32"/>
-      <c r="E36" s="32"/>
-      <c r="F36" s="32"/>
-      <c r="G36" s="32"/>
-      <c r="H36" s="32"/>
-      <c r="I36" s="32"/>
-      <c r="J36" s="32"/>
-      <c r="K36" s="32"/>
-      <c r="L36" s="32"/>
-      <c r="M36" s="32"/>
-      <c r="N36" s="32"/>
-      <c r="O36" s="32"/>
+      <c r="D36" s="33"/>
+      <c r="E36" s="33"/>
+      <c r="F36" s="33"/>
+      <c r="G36" s="33"/>
+      <c r="H36" s="33"/>
+      <c r="I36" s="33"/>
+      <c r="J36" s="33"/>
+      <c r="K36" s="33"/>
+      <c r="L36" s="33"/>
+      <c r="M36" s="33"/>
+      <c r="N36" s="33"/>
+      <c r="O36" s="33"/>
       <c r="P36" s="20" t="s">
         <v>39</v>
       </c>
@@ -2252,24 +2258,24 @@
       <c r="T36" s="20"/>
       <c r="U36" s="20"/>
       <c r="V36" s="20"/>
-      <c r="W36" s="33"/>
-      <c r="X36" s="34" t="n">
-        <v>45770</v>
-      </c>
-      <c r="Y36" s="34"/>
-      <c r="Z36" s="34"/>
-      <c r="AA36" s="34"/>
-      <c r="AB36" s="34"/>
-      <c r="AC36" s="34"/>
-      <c r="AD36" s="34"/>
-      <c r="AE36" s="33"/>
-      <c r="AF36" s="34" t="n">
-        <v>46022</v>
-      </c>
-      <c r="AG36" s="34"/>
-      <c r="AH36" s="34"/>
-      <c r="AI36" s="34"/>
-      <c r="AJ36" s="34"/>
+      <c r="W36" s="34"/>
+      <c r="X36" s="35" t="n">
+        <v>46017</v>
+      </c>
+      <c r="Y36" s="35"/>
+      <c r="Z36" s="35"/>
+      <c r="AA36" s="35"/>
+      <c r="AB36" s="35"/>
+      <c r="AC36" s="35"/>
+      <c r="AD36" s="35"/>
+      <c r="AE36" s="34"/>
+      <c r="AF36" s="35" t="n">
+        <v>46260</v>
+      </c>
+      <c r="AG36" s="35"/>
+      <c r="AH36" s="35"/>
+      <c r="AI36" s="35"/>
+      <c r="AJ36" s="35"/>
     </row>
     <row r="37" customFormat="false" ht="6.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="38" customFormat="false" ht="6.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2289,147 +2295,147 @@
       <c r="M39" s="19"/>
       <c r="N39" s="19"/>
       <c r="O39" s="19"/>
-      <c r="P39" s="35" t="s">
+      <c r="P39" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="Q39" s="35"/>
-      <c r="R39" s="35"/>
-      <c r="S39" s="35"/>
-      <c r="T39" s="35"/>
-      <c r="U39" s="35"/>
-      <c r="V39" s="35"/>
-      <c r="W39" s="35"/>
-      <c r="X39" s="35"/>
-      <c r="Y39" s="35"/>
-      <c r="Z39" s="35"/>
-      <c r="AA39" s="35"/>
-      <c r="AB39" s="35"/>
-      <c r="AC39" s="35"/>
-      <c r="AD39" s="35"/>
-      <c r="AE39" s="35"/>
-      <c r="AF39" s="35"/>
-      <c r="AG39" s="35"/>
-      <c r="AH39" s="35"/>
-      <c r="AI39" s="35"/>
-      <c r="AJ39" s="35"/>
+      <c r="Q39" s="28"/>
+      <c r="R39" s="28"/>
+      <c r="S39" s="28"/>
+      <c r="T39" s="28"/>
+      <c r="U39" s="28"/>
+      <c r="V39" s="28"/>
+      <c r="W39" s="28"/>
+      <c r="X39" s="28"/>
+      <c r="Y39" s="28"/>
+      <c r="Z39" s="28"/>
+      <c r="AA39" s="28"/>
+      <c r="AB39" s="28"/>
+      <c r="AC39" s="28"/>
+      <c r="AD39" s="28"/>
+      <c r="AE39" s="28"/>
+      <c r="AF39" s="28"/>
+      <c r="AG39" s="28"/>
+      <c r="AH39" s="28"/>
+      <c r="AI39" s="28"/>
+      <c r="AJ39" s="28"/>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C40" s="28" t="s">
+      <c r="C40" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="D40" s="28"/>
-      <c r="E40" s="28"/>
-      <c r="F40" s="28"/>
-      <c r="G40" s="28"/>
-      <c r="H40" s="28"/>
-      <c r="I40" s="28"/>
-      <c r="J40" s="28"/>
-      <c r="K40" s="28"/>
-      <c r="L40" s="28"/>
-      <c r="M40" s="28"/>
-      <c r="N40" s="29"/>
-      <c r="P40" s="35"/>
-      <c r="Q40" s="35"/>
-      <c r="R40" s="35"/>
-      <c r="S40" s="35"/>
-      <c r="T40" s="35"/>
-      <c r="U40" s="35"/>
-      <c r="V40" s="35"/>
-      <c r="W40" s="35"/>
-      <c r="X40" s="35"/>
-      <c r="Y40" s="35"/>
-      <c r="Z40" s="35"/>
-      <c r="AA40" s="35"/>
-      <c r="AB40" s="35"/>
-      <c r="AC40" s="35"/>
-      <c r="AD40" s="35"/>
-      <c r="AE40" s="35"/>
-      <c r="AF40" s="35"/>
-      <c r="AG40" s="35"/>
-      <c r="AH40" s="35"/>
-      <c r="AI40" s="35"/>
-      <c r="AJ40" s="35"/>
+      <c r="D40" s="29"/>
+      <c r="E40" s="29"/>
+      <c r="F40" s="29"/>
+      <c r="G40" s="29"/>
+      <c r="H40" s="29"/>
+      <c r="I40" s="29"/>
+      <c r="J40" s="29"/>
+      <c r="K40" s="29"/>
+      <c r="L40" s="29"/>
+      <c r="M40" s="29"/>
+      <c r="N40" s="30"/>
+      <c r="P40" s="28"/>
+      <c r="Q40" s="28"/>
+      <c r="R40" s="28"/>
+      <c r="S40" s="28"/>
+      <c r="T40" s="28"/>
+      <c r="U40" s="28"/>
+      <c r="V40" s="28"/>
+      <c r="W40" s="28"/>
+      <c r="X40" s="28"/>
+      <c r="Y40" s="28"/>
+      <c r="Z40" s="28"/>
+      <c r="AA40" s="28"/>
+      <c r="AB40" s="28"/>
+      <c r="AC40" s="28"/>
+      <c r="AD40" s="28"/>
+      <c r="AE40" s="28"/>
+      <c r="AF40" s="28"/>
+      <c r="AG40" s="28"/>
+      <c r="AH40" s="28"/>
+      <c r="AI40" s="28"/>
+      <c r="AJ40" s="28"/>
     </row>
     <row r="41" customFormat="false" ht="53.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C41" s="28"/>
-      <c r="D41" s="28"/>
-      <c r="E41" s="28"/>
-      <c r="F41" s="28"/>
-      <c r="G41" s="28"/>
-      <c r="H41" s="28"/>
-      <c r="I41" s="28"/>
-      <c r="J41" s="28"/>
-      <c r="K41" s="28"/>
-      <c r="L41" s="28"/>
-      <c r="M41" s="28"/>
-      <c r="N41" s="29"/>
-      <c r="P41" s="35"/>
-      <c r="Q41" s="35"/>
-      <c r="R41" s="35"/>
-      <c r="S41" s="35"/>
-      <c r="T41" s="35"/>
-      <c r="U41" s="35"/>
-      <c r="V41" s="35"/>
-      <c r="W41" s="35"/>
-      <c r="X41" s="35"/>
-      <c r="Y41" s="35"/>
-      <c r="Z41" s="35"/>
-      <c r="AA41" s="35"/>
-      <c r="AB41" s="35"/>
-      <c r="AC41" s="35"/>
-      <c r="AD41" s="35"/>
-      <c r="AE41" s="35"/>
-      <c r="AF41" s="35"/>
-      <c r="AG41" s="35"/>
-      <c r="AH41" s="35"/>
-      <c r="AI41" s="35"/>
-      <c r="AJ41" s="35"/>
+      <c r="C41" s="29"/>
+      <c r="D41" s="29"/>
+      <c r="E41" s="29"/>
+      <c r="F41" s="29"/>
+      <c r="G41" s="29"/>
+      <c r="H41" s="29"/>
+      <c r="I41" s="29"/>
+      <c r="J41" s="29"/>
+      <c r="K41" s="29"/>
+      <c r="L41" s="29"/>
+      <c r="M41" s="29"/>
+      <c r="N41" s="30"/>
+      <c r="P41" s="28"/>
+      <c r="Q41" s="28"/>
+      <c r="R41" s="28"/>
+      <c r="S41" s="28"/>
+      <c r="T41" s="28"/>
+      <c r="U41" s="28"/>
+      <c r="V41" s="28"/>
+      <c r="W41" s="28"/>
+      <c r="X41" s="28"/>
+      <c r="Y41" s="28"/>
+      <c r="Z41" s="28"/>
+      <c r="AA41" s="28"/>
+      <c r="AB41" s="28"/>
+      <c r="AC41" s="28"/>
+      <c r="AD41" s="28"/>
+      <c r="AE41" s="28"/>
+      <c r="AF41" s="28"/>
+      <c r="AG41" s="28"/>
+      <c r="AH41" s="28"/>
+      <c r="AI41" s="28"/>
+      <c r="AJ41" s="28"/>
     </row>
     <row r="42" customFormat="false" ht="42" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="P42" s="35"/>
-      <c r="Q42" s="35"/>
-      <c r="R42" s="35"/>
-      <c r="S42" s="35"/>
-      <c r="T42" s="35"/>
-      <c r="U42" s="35"/>
-      <c r="V42" s="35"/>
-      <c r="W42" s="35"/>
-      <c r="X42" s="35"/>
-      <c r="Y42" s="35"/>
-      <c r="Z42" s="35"/>
-      <c r="AA42" s="35"/>
-      <c r="AB42" s="35"/>
-      <c r="AC42" s="35"/>
-      <c r="AD42" s="35"/>
-      <c r="AE42" s="35"/>
-      <c r="AF42" s="35"/>
-      <c r="AG42" s="35"/>
-      <c r="AH42" s="35"/>
-      <c r="AI42" s="35"/>
-      <c r="AJ42" s="35"/>
+      <c r="P42" s="28"/>
+      <c r="Q42" s="28"/>
+      <c r="R42" s="28"/>
+      <c r="S42" s="28"/>
+      <c r="T42" s="28"/>
+      <c r="U42" s="28"/>
+      <c r="V42" s="28"/>
+      <c r="W42" s="28"/>
+      <c r="X42" s="28"/>
+      <c r="Y42" s="28"/>
+      <c r="Z42" s="28"/>
+      <c r="AA42" s="28"/>
+      <c r="AB42" s="28"/>
+      <c r="AC42" s="28"/>
+      <c r="AD42" s="28"/>
+      <c r="AE42" s="28"/>
+      <c r="AF42" s="28"/>
+      <c r="AG42" s="28"/>
+      <c r="AH42" s="28"/>
+      <c r="AI42" s="28"/>
+      <c r="AJ42" s="28"/>
     </row>
     <row r="43" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="P43" s="35"/>
-      <c r="Q43" s="35"/>
-      <c r="R43" s="35"/>
-      <c r="S43" s="35"/>
-      <c r="T43" s="35"/>
-      <c r="U43" s="35"/>
-      <c r="V43" s="35"/>
-      <c r="W43" s="35"/>
-      <c r="X43" s="35"/>
-      <c r="Y43" s="35"/>
-      <c r="Z43" s="35"/>
-      <c r="AA43" s="35"/>
-      <c r="AB43" s="35"/>
-      <c r="AC43" s="35"/>
-      <c r="AD43" s="35"/>
-      <c r="AE43" s="35"/>
-      <c r="AF43" s="35"/>
-      <c r="AG43" s="35"/>
-      <c r="AH43" s="35"/>
-      <c r="AI43" s="35"/>
-      <c r="AJ43" s="35"/>
+      <c r="P43" s="28"/>
+      <c r="Q43" s="28"/>
+      <c r="R43" s="28"/>
+      <c r="S43" s="28"/>
+      <c r="T43" s="28"/>
+      <c r="U43" s="28"/>
+      <c r="V43" s="28"/>
+      <c r="W43" s="28"/>
+      <c r="X43" s="28"/>
+      <c r="Y43" s="28"/>
+      <c r="Z43" s="28"/>
+      <c r="AA43" s="28"/>
+      <c r="AB43" s="28"/>
+      <c r="AC43" s="28"/>
+      <c r="AD43" s="28"/>
+      <c r="AE43" s="28"/>
+      <c r="AF43" s="28"/>
+      <c r="AG43" s="28"/>
+      <c r="AH43" s="28"/>
+      <c r="AI43" s="28"/>
+      <c r="AJ43" s="28"/>
     </row>
     <row r="44" customFormat="false" ht="6.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="45" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3174,9 +3180,6 @@
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
-  <hyperlinks>
-    <hyperlink ref="P29" r:id="rId1" display="https://webservicesexternos.banagricola.com:9443"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.736111111111111" bottom="0.75" header="0.3" footer="0.511811023622047"/>
   <pageSetup paperSize="1" scale="88" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -3184,6 +3187,6 @@
     <oddHeader>&amp;L&amp;10 Grupo Bancolombia Clasificación – Interna&amp;1#_x005F_x000D_</oddHeader>
     <oddFooter/>
   </headerFooter>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>